<commit_message>
Adicionado data de controle
</commit_message>
<xml_diff>
--- a/kanban_com_subtarefas.xlsx
+++ b/kanban_com_subtarefas.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -459,6 +459,16 @@
           <t>Subtarefas</t>
         </is>
       </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>DataCriacao</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>DataModificacao</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -486,6 +496,8 @@
           <t>Ler sobre contratos inteligentes:False;Criar exemplo em Solidity:False</t>
         </is>
       </c>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -513,6 +525,8 @@
           <t>Revisar fundamentos:False;Fazer projetos práticos:False</t>
         </is>
       </c>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -540,6 +554,8 @@
           <t>Fazer exercícios avançados:False;Criar scripts úteis:False</t>
         </is>
       </c>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -567,6 +583,8 @@
           <t>Estudar ownership:False;Criar CLI básica:False</t>
         </is>
       </c>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -594,6 +612,8 @@
           <t>Estudar goroutines:False;Desenvolver microserviço:False</t>
         </is>
       </c>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -621,6 +641,8 @@
           <t>Conversação semanal:False;Assistir conteúdo técnico:False</t>
         </is>
       </c>
+      <c r="F7" t="inlineStr"/>
+      <c r="G7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -648,6 +670,8 @@
           <t>Revisar vocabulário:False;Estudar gramática:False</t>
         </is>
       </c>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -675,6 +699,8 @@
           <t>Leitura de textos:False</t>
         </is>
       </c>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -702,6 +728,8 @@
           <t>Ler textos clássicos:False</t>
         </is>
       </c>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -729,6 +757,8 @@
           <t>Aprender tons básicos:False</t>
         </is>
       </c>
+      <c r="F11" t="inlineStr"/>
+      <c r="G11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -756,6 +786,8 @@
           <t>Revisar backend:False;Subir nova versão:False</t>
         </is>
       </c>
+      <c r="F12" t="inlineStr"/>
+      <c r="G12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -783,6 +815,8 @@
           <t>Testar controle de entrada/saída:False</t>
         </is>
       </c>
+      <c r="F13" t="inlineStr"/>
+      <c r="G13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -810,6 +844,8 @@
           <t>Gerar algoritmo aleatório:False</t>
         </is>
       </c>
+      <c r="F14" t="inlineStr"/>
+      <c r="G14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -837,6 +873,8 @@
           <t>Converter PDF em cifra:False</t>
         </is>
       </c>
+      <c r="F15" t="inlineStr"/>
+      <c r="G15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -864,6 +902,8 @@
           <t>Adicionar plano alimentar:False</t>
         </is>
       </c>
+      <c r="F16" t="inlineStr"/>
+      <c r="G16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -891,6 +931,8 @@
           <t>Monitorar carteira:False</t>
         </is>
       </c>
+      <c r="F17" t="inlineStr"/>
+      <c r="G17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -918,6 +960,8 @@
           <t>Organizar repertório:False;Gravar 1ª faixa:False</t>
         </is>
       </c>
+      <c r="F18" t="inlineStr"/>
+      <c r="G18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -945,6 +989,8 @@
           <t>Pozzoli e Suzuki:False;Teoria elementar:False</t>
         </is>
       </c>
+      <c r="F19" t="inlineStr"/>
+      <c r="G19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -972,6 +1018,8 @@
           <t>Rotina semanal de estudo:False</t>
         </is>
       </c>
+      <c r="F20" t="inlineStr"/>
+      <c r="G20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -999,6 +1047,8 @@
           <t>Treinar repertório:False</t>
         </is>
       </c>
+      <c r="F21" t="inlineStr"/>
+      <c r="G21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1024,6 +1074,45 @@
       <c r="E22" t="inlineStr">
         <is>
           <t>Planejar vídeos semanais:False;Gravar episódio 1:False</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr"/>
+      <c r="G22" t="inlineStr"/>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Mestre do Capitalismo</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>A FAZER</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Finanças</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Alta</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>copiar videos:False</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>2025-04-16 21:43:05</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>2025-04-16 21:43:05</t>
         </is>
       </c>
     </row>

</xml_diff>